<commit_message>
Changed how the records are displayed on the results.txt file
</commit_message>
<xml_diff>
--- a/nfl_odds_analysis/nfl_odds.xlsx
+++ b/nfl_odds_analysis/nfl_odds.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="180" yWindow="460" windowWidth="25420" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="C266" sqref="C266"/>
+    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
+      <selection activeCell="B266" sqref="B266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7318,13 +7318,13 @@
         <v>13</v>
       </c>
       <c r="B265">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C265" t="s">
         <v>18</v>
       </c>
       <c r="D265">
-        <v>-153</v>
+        <v>-154</v>
       </c>
       <c r="E265">
         <v>0</v>
@@ -7344,13 +7344,13 @@
         <v>30</v>
       </c>
       <c r="B266">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="C266" t="s">
         <v>15</v>
       </c>
       <c r="D266">
-        <v>-178</v>
+        <v>-172</v>
       </c>
       <c r="E266">
         <v>0</v>

</xml_diff>

<commit_message>
Added the calculation of records as favorites and underdogs
</commit_message>
<xml_diff>
--- a/nfl_odds_analysis/nfl_odds.xlsx
+++ b/nfl_odds_analysis/nfl_odds.xlsx
@@ -440,7 +440,7 @@
   <dimension ref="A1:H266"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
-      <selection activeCell="B266" sqref="B266"/>
+      <selection activeCell="D265" sqref="D265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7344,13 +7344,13 @@
         <v>30</v>
       </c>
       <c r="B266">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C266" t="s">
         <v>15</v>
       </c>
       <c r="D266">
-        <v>-172</v>
+        <v>-167</v>
       </c>
       <c r="E266">
         <v>0</v>

</xml_diff>

<commit_message>
added the conference championship game scores and fixed a bug in the ATS calculator
</commit_message>
<xml_diff>
--- a/nfl_odds_analysis/nfl_odds.xlsx
+++ b/nfl_odds_analysis/nfl_odds.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="32">
   <si>
     <t>Atlanta</t>
   </si>
@@ -437,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H266"/>
+  <dimension ref="A1:H267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
-      <selection activeCell="D265" sqref="D265"/>
+    <sheetView tabSelected="1" topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="B268" sqref="B268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7315,22 +7315,22 @@
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="B265">
         <v>139</v>
       </c>
       <c r="C265" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D265">
         <v>-154</v>
       </c>
       <c r="E265">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F265">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="G265">
         <v>3</v>
@@ -7341,28 +7341,54 @@
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
+        <v>13</v>
+      </c>
+      <c r="B266">
+        <v>154</v>
+      </c>
+      <c r="C266" t="s">
+        <v>18</v>
+      </c>
+      <c r="D266">
+        <v>-171</v>
+      </c>
+      <c r="E266">
+        <v>37</v>
+      </c>
+      <c r="F266">
+        <v>31</v>
+      </c>
+      <c r="G266">
+        <v>3</v>
+      </c>
+      <c r="H266">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>13</v>
+      </c>
+      <c r="B267">
+        <v>-127</v>
+      </c>
+      <c r="C267" t="s">
         <v>30</v>
       </c>
-      <c r="B266">
-        <v>151</v>
-      </c>
-      <c r="C266" t="s">
-        <v>15</v>
-      </c>
-      <c r="D266">
-        <v>-167</v>
-      </c>
-      <c r="E266">
+      <c r="D267">
+        <v>115</v>
+      </c>
+      <c r="E267">
         <v>0</v>
       </c>
-      <c r="F266">
+      <c r="F267">
         <v>0</v>
       </c>
-      <c r="G266">
-        <v>3.5</v>
-      </c>
-      <c r="H266">
-        <v>-3.5</v>
+      <c r="G267">
+        <v>-1.5</v>
+      </c>
+      <c r="H267">
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>